<commit_message>
Update View Berkas RKA & Regulasi
All Done
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
+++ b/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDM\RAPAT\RAPAT KOORDINASI SISTEM SDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05525651-27A6-468A-92EE-2E9AC5970A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tahap 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Tahap 3" sheetId="6" r:id="rId3"/>
     <sheet name="Tahap 4" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Rencana Sistem SDM</t>
   </si>
@@ -308,14 +308,6 @@
     <t>menu upload SPK dan RKK (di isi oleh komite keperawatan, komite nakesla dan komite medik) masuk di biodata pegawai
 a. Upload SPK (Surat Penugasan Klinis) dan RKK (rincian kewenangan klinis) pdf ada riwayat
 b. Share di pegawai terkait</t>
-  </si>
-  <si>
-    <t>pengajuan cuti, jadwal unit, ijin sakit upload surat ijin sakit verif atasan, kepeg
-a. Mengisi jadwal unit yang di verifikasi oleh  manajer terkait / Kasubag/ Kabag/ dan Kabag kepegawaian (jika ditolak diberikan keterangan alasan ditolak)
-b. Pengajuan cuti tahunan oleh masing2 pegawai yang di verif oleh atasan, rekan delegasi (jika ada),  Kabag kepegawaian
-c. Pengajuan cuti melahirkan (verifikasi atasan dan upload surat pengajuan cuti melahirkan) bisa d edit oleh pegawai (perubahan)
-d. Ijin sakit (verif atasan, kepegawaian dan upload surat ijin)
-e. Rekap masing2 pegawai jumlah ijin dan cuti setiap bulannya dan 1 tahun.</t>
   </si>
   <si>
     <t>menu sselesai perjalanan dinas
@@ -339,11 +331,25 @@
     - Lain2 (mengisi manual)
 Ada tracking pengajuannya</t>
   </si>
+  <si>
+    <t>semua nakes punya sip dan str (kalo seumur hidup hanya input nomor str),</t>
+  </si>
+  <si>
+    <t>pengajuan jadwal setelah ditolak dari atasan langsung akan tampil alasan penolakan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jadwal unit... pengajuan cuti, ijin sakit upload surat ijin sakit verif atasan, kepeg
+a. Mengisi jadwal unit yang di verifikasi oleh  manajer terkait / Kasubag/ Kabag/ dan Kabag kepegawaian (jika ditolak diberikan keterangan alasan ditolak)
+b. Pengajuan cuti tahunan oleh masing2 pegawai yang di verif oleh atasan, rekan delegasi (jika ada),  Kabag kepegawaian
+c. Pengajuan cuti melahirkan (verifikasi atasan dan upload surat pengajuan cuti melahirkan) bisa d edit oleh pegawai (perubahan)
+d. Ijin sakit (verif atasan, kepegawaian dan upload surat ijin)
+e. Rekap masing2 pegawai jumlah ijin dan cuti setiap bulannya atau per tahunnya</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -442,13 +448,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,26 +768,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="108.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" style="8" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -793,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -803,8 +809,11 @@
       <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -815,7 +824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -826,7 +835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -837,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -848,18 +857,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -870,11 +879,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -888,25 +897,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="125.7109375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="61.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -917,29 +927,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="D5" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -950,7 +963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -961,7 +974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -972,7 +985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -983,12 +996,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+    <row r="11" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>10</v>
@@ -1001,56 +1014,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView zoomScale="119" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="136.140625" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="126" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C9"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="131" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1076,6 +1043,52 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="131" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="136.140625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
@@ -1124,10 +1137,10 @@
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update View Profil Karyawan
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
+++ b/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05525651-27A6-468A-92EE-2E9AC5970A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26841ED-0E36-46E2-9F53-04C965FA2AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tahap 1" sheetId="1" r:id="rId1"/>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -879,7 +879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -900,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Udd Table Referensi and Starting to edit Profil Document
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
+++ b/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26841ED-0E36-46E2-9F53-04C965FA2AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0340CAD-10A4-470F-B3D7-DBEC0963D840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,9 @@
     <sheet name="Tahap 3" sheetId="6" r:id="rId3"/>
     <sheet name="Tahap 4" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tahap 1'!$A$1:$D$20,'Tahap 1'!$A$22:$C$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
-  <si>
-    <t>Rencana Sistem SDM</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -332,9 +332,6 @@
 Ada tracking pengajuannya</t>
   </si>
   <si>
-    <t>semua nakes punya sip dan str (kalo seumur hidup hanya input nomor str),</t>
-  </si>
-  <si>
     <t>pengajuan jadwal setelah ditolak dari atasan langsung akan tampil alasan penolakan</t>
   </si>
   <si>
@@ -344,6 +341,18 @@
 c. Pengajuan cuti melahirkan (verifikasi atasan dan upload surat pengajuan cuti melahirkan) bisa d edit oleh pegawai (perubahan)
 d. Ijin sakit (verif atasan, kepegawaian dan upload surat ijin)
 e. Rekap masing2 pegawai jumlah ijin dan cuti setiap bulannya atau per tahunnya</t>
+  </si>
+  <si>
+    <t>Rencana Sistem SDM Tahap 2 Profil Pegawai</t>
+  </si>
+  <si>
+    <t>Rencana Sistem SDM Tahap 3 Profil Pegawai</t>
+  </si>
+  <si>
+    <t>Rencana Sistem SDM Tahap 4 Profil Pegawai</t>
+  </si>
+  <si>
+    <t>semua nakes punya sip dan str (kalo seumur hidup hanya input nomor str)</t>
   </si>
 </sst>
 </file>
@@ -405,7 +414,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -428,13 +437,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,6 +471,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,380 +792,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G12"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="108.7109375" customWidth="1"/>
+    <col min="2" max="2" width="116.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="8" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="8"/>
+    <col min="4" max="4" width="13" style="7" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>7</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    </row>
+    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="C29" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>4</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>8</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="B32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="10000" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A26:C26"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="14" scale="63" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="125.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="61.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>10</v>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="10000" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="14" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="136.140625" customWidth="1"/>
+    <col min="2" max="2" width="102.140625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="126" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="131" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="136.140625" customWidth="1"/>
+    <col min="2" max="2" width="75.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1</v>
+      <c r="A5" s="2">
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>3</v>
+      <c r="A7" s="2">
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="C7" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Form Batal Rotasi done
minus Ubah NIP & download dokumen str sip
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
+++ b/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0340CAD-10A4-470F-B3D7-DBEC0963D840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D8551F-3682-49E8-AC45-541AEC946B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,11 +472,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,8 +797,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,11 +810,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -919,11 +919,11 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1025,11 +1025,11 @@
       <c r="D20" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1054,17 +1054,17 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1153,11 +1153,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1275,11 +1275,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1326,17 +1326,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">

</xml_diff>

<commit_message>
Update View Menu Kepegawaian
done. minus Hapus Akun
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
+++ b/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D8551F-3682-49E8-AC45-541AEC946B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AE0962-D39C-411C-9F77-3E030AA04CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,11 +305,6 @@
 g. Rekap pegawai berlaku str,sip, btcls/atcls</t>
   </si>
   <si>
-    <t>menu upload SPK dan RKK (di isi oleh komite keperawatan, komite nakesla dan komite medik) masuk di biodata pegawai
-a. Upload SPK (Surat Penugasan Klinis) dan RKK (rincian kewenangan klinis) pdf ada riwayat
-b. Share di pegawai terkait</t>
-  </si>
-  <si>
     <t>menu sselesai perjalanan dinas
 1. cheklist surat tugas
 2. cheklist nama petugas yang berangkat
@@ -353,6 +348,13 @@
   </si>
   <si>
     <t>semua nakes punya sip dan str (kalo seumur hidup hanya input nomor str)</t>
+  </si>
+  <si>
+    <t>menu upload SPK dan RKK (di isi oleh komite keperawatan, komite nakesla dan komite medik) masuk di biodata pegawai
+a. Upload SPK (Surat Penugasan Klinis) dan RKK (rincian kewenangan klinis) pdf ada riwayat
+b. Share di pegawai terkait
+c. tgl berakhir SPK kontrak &amp; thl
+d. notifikasi 3 bulan sebelum SPK habis</t>
   </si>
 </sst>
 </file>
@@ -798,7 +800,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +840,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -907,12 +909,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>7</v>
@@ -920,7 +922,7 @@
     </row>
     <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -943,13 +945,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
@@ -957,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>9</v>
@@ -1017,7 +1019,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>9</v>
@@ -1026,7 +1028,7 @@
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -1055,7 +1057,7 @@
     </row>
     <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1154,7 +1156,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1175,13 +1177,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
@@ -1189,7 +1191,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>9</v>
@@ -1244,7 +1246,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>9</v>
@@ -1276,7 +1278,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1327,7 +1329,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>

</xml_diff>

<commit_message>
Adding SPK RKK Done
fix bug in datalogs
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
+++ b/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AE0962-D39C-411C-9F77-3E030AA04CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD80B5F9-16D5-4AE9-922A-5F76DE06EA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -800,7 +800,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Open Working - TAHAP 2
</commit_message>
<xml_diff>
--- a/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
+++ b/project/kepegawaian/Rapat Koordinasi Sistem SDM Tahap 1 (Profil Pegawai).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\kepegawaian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD80B5F9-16D5-4AE9-922A-5F76DE06EA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51254A0C-16BA-4340-B1ED-5E8BD6B1DE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tahap 1" sheetId="1" r:id="rId1"/>
@@ -799,7 +799,7 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:D9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1267,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>